<commit_message>
Baseball: Working on displaying all of the algorithm frame and real frame
</commit_message>
<xml_diff>
--- a/Baseball Catcher/baseball_catcher_trial_runs.xlsx
+++ b/Baseball Catcher/baseball_catcher_trial_runs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Catch</t>
   </si>
@@ -32,6 +32,21 @@
   </si>
   <si>
     <t>Uncatchable</t>
+  </si>
+  <si>
+    <t>catch = 4</t>
+  </si>
+  <si>
+    <t>rim = 2</t>
+  </si>
+  <si>
+    <t>miss = 0</t>
+  </si>
+  <si>
+    <t>uncatchable = x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -385,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection sqref="A1:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -523,10 +538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -535,9 +550,10 @@
     <col min="2" max="2" width="3.734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.26171875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.9453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,6 +565,29 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Baseball: Saved off HardWare.cpp used to get 60 points
</commit_message>
<xml_diff>
--- a/Baseball Catcher/baseball_catcher_trial_runs.xlsx
+++ b/Baseball Catcher/baseball_catcher_trial_runs.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="1" r:id="rId1"/>
     <sheet name="Run 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Catch</t>
   </si>
@@ -47,6 +47,18 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>11 catches</t>
+  </si>
+  <si>
+    <t>8 rims</t>
+  </si>
+  <si>
+    <t>1 miss</t>
+  </si>
+  <si>
+    <t>1 uncatchable</t>
   </si>
 </sst>
 </file>
@@ -398,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -412,91 +424,115 @@
     <col min="4" max="4" width="10.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1">
+        <f>SUM(A3:A23)*4</f>
+        <v>44</v>
+      </c>
+      <c r="B1">
+        <f>SUM(B3:B23)*2</f>
+        <v>16</v>
+      </c>
+      <c r="C1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1">
+        <f>SUM(A1:B1)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B16">
         <v>1</v>
       </c>
@@ -507,12 +543,12 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18">
+      <c r="B18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
+      <c r="C19">
         <v>1</v>
       </c>
     </row>
@@ -522,12 +558,17 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="D21">
+      <c r="A21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
         <v>1</v>
       </c>
     </row>
@@ -540,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -571,16 +612,25 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>

</xml_diff>